<commit_message>
Revise excel template structure
</commit_message>
<xml_diff>
--- a/excel/templates/template_en.xlsx
+++ b/excel/templates/template_en.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24931"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hj-micro\regslv\parser\excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FB1CDB6-D6A2-4A02-BC3C-38E53E167041}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D87158B9-C3B8-4918-953B-FBB6A5FC487B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="852" yWindow="1440" windowWidth="24408" windowHeight="15120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5100" yWindow="1908" windowWidth="22776" windowHeight="14652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEM" sheetId="1" r:id="rId1"/>
@@ -25,20 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="36">
-  <si>
-    <t>0X00</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>TEM</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>RW</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>0X00000000</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -51,10 +43,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>0</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>0x0</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -67,10 +55,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>0,1</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>16:14</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -95,10 +79,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>0~7</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>12:0</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -107,26 +87,14 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Base Address</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Address Offset</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Length</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Abbreviation</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Access Type</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Description</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -143,19 +111,11 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>Access Type</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>Reset Value</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Reset Signal</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
-    <t>Optional Value</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
@@ -173,6 +133,58 @@
   </si>
   <si>
     <t>Template Register</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Width</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>Read Type</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>R</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>W</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RCLR</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>NA</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RSET</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>WOSET</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>RUSER</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>WOT</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>R</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>W</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Write Type</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -285,7 +297,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -298,7 +310,6 @@
     <xf numFmtId="49" fontId="5" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="5" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -591,7 +602,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -605,36 +616,36 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B1" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7"/>
+        <v>14</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
+        <v>15</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="6"/>
+      <c r="D2" s="6"/>
+      <c r="E2" s="6"/>
+      <c r="F2" s="6"/>
+      <c r="G2" s="6"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>0</v>
+        <v>26</v>
+      </c>
+      <c r="B3" s="7">
+        <v>32</v>
       </c>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -644,206 +655,175 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="B4" s="8">
-        <v>32</v>
-      </c>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
+        <v>16</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C5" s="6"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="6"/>
+      <c r="F5" s="6"/>
+      <c r="G5" s="6"/>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="7" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="7"/>
-      <c r="D5" s="7"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="7"/>
-      <c r="G5" s="7"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="s">
+      <c r="D10" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="4" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C11" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B6" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="7"/>
-      <c r="E6" s="7"/>
-      <c r="F6" s="7"/>
-      <c r="G6" s="7"/>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B7" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C7" s="7"/>
-      <c r="D7" s="7"/>
-      <c r="E7" s="7"/>
-      <c r="F7" s="7"/>
-      <c r="G7" s="7"/>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="3" t="s">
+      <c r="D11" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
+      <c r="E11" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F11" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C11" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D11" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>7</v>
-      </c>
       <c r="G11" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>33</v>
+        <v>23</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>2</v>
+        <v>35</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C13" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="D13" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E13" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G13" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C14" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="C16" s="6"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="B7:G7"/>
+  <mergeCells count="5">
+    <mergeCell ref="B5:G5"/>
+    <mergeCell ref="B1:G1"/>
     <mergeCell ref="B2:G2"/>
-    <mergeCell ref="B1:G1"/>
     <mergeCell ref="B3:G3"/>
     <mergeCell ref="B4:G4"/>
-    <mergeCell ref="B5:G5"/>
-    <mergeCell ref="B6:G6"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>